<commit_message>
[FIX] ports exception rule
</commit_message>
<xml_diff>
--- a/Comparator_Reports/Excel_Comparator/24_03_001_validation_log.xlsx
+++ b/Comparator_Reports/Excel_Comparator/24_03_001_validation_log.xlsx
@@ -834,240 +834,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004FF20ACD2ACDAF4B84EF9300C67B2159" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0c36ae600cfc71a682facb2fe9ea4a9f">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1e4be601-d1eb-4833-8855-b10f66ff5f6e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="efc49a46b45dba0aa538c93634f147fb" ns2:_="">
-    <xsd:import namespace="1e4be601-d1eb-4833-8855-b10f66ff5f6e"/>
-    <xsd:element name="properties">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element name="documentManagement">
-            <xsd:complexType>
-              <xsd:all>
-                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
-                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
-                <xsd:element ref="ns2:Owner"/>
-              </xsd:all>
-            </xsd:complexType>
-          </xsd:element>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="1e4be601-d1eb-4833-8855-b10f66ff5f6e" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceSearchProperties" ma:index="10" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="11" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="13" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="111f8b2a-cd79-47dd-889c-3fa2f1862339" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="MediaServiceDateTaken" ma:index="14" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceOCR" ma:index="15" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceGenerationTime" ma:index="16" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceEventHashCode" ma:index="17" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="Owner" ma:index="18" ma:displayName="Owner" ma:format="Dropdown" ma:list="UserInfo" ma:SharePointGroup="0" ma:internalName="Owner">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:UserMulti">
-            <xsd:sequence>
-              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
-                <xsd:complexType>
-                  <xsd:sequence>
-                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
-                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0"/>
-                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
-                  </xsd:sequence>
-                </xsd:complexType>
-              </xsd:element>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
-    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
-    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
-    <xsd:element name="coreProperties" type="CT_coreProperties"/>
-    <xsd:complexType name="CT_coreProperties">
-      <xsd:all>
-        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
-        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
-          <xsd:annotation>
-            <xsd:documentation>
-                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
-                    </xsd:documentation>
-          </xsd:annotation>
-        </xsd:element>
-        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-      </xsd:all>
-    </xsd:complexType>
-  </xsd:schema>
-  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
-    <xs:element name="Person">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:DisplayName" minOccurs="0"/>
-          <xs:element ref="pc:AccountId" minOccurs="0"/>
-          <xs:element ref="pc:AccountType" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="DisplayName" type="xs:string"/>
-    <xs:element name="AccountId" type="xs:string"/>
-    <xs:element name="AccountType" type="xs:string"/>
-    <xs:element name="BDCAssociatedEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-        <xs:attribute ref="pc:EntityNamespace"/>
-        <xs:attribute ref="pc:EntityName"/>
-        <xs:attribute ref="pc:SystemInstanceName"/>
-        <xs:attribute ref="pc:AssociationName"/>
-      </xs:complexType>
-    </xs:element>
-    <xs:attribute name="EntityNamespace" type="xs:string"/>
-    <xs:attribute name="EntityName" type="xs:string"/>
-    <xs:attribute name="SystemInstanceName" type="xs:string"/>
-    <xs:attribute name="AssociationName" type="xs:string"/>
-    <xs:element name="BDCEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
-          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
-          <xs:element ref="pc:EntityId1" minOccurs="0"/>
-          <xs:element ref="pc:EntityId2" minOccurs="0"/>
-          <xs:element ref="pc:EntityId3" minOccurs="0"/>
-          <xs:element ref="pc:EntityId4" minOccurs="0"/>
-          <xs:element ref="pc:EntityId5" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="EntityDisplayName" type="xs:string"/>
-    <xs:element name="EntityInstanceReference" type="xs:string"/>
-    <xs:element name="EntityId1" type="xs:string"/>
-    <xs:element name="EntityId2" type="xs:string"/>
-    <xs:element name="EntityId3" type="xs:string"/>
-    <xs:element name="EntityId4" type="xs:string"/>
-    <xs:element name="EntityId5" type="xs:string"/>
-    <xs:element name="Terms">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermInfo">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermName" minOccurs="0"/>
-          <xs:element ref="pc:TermId" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermName" type="xs:string"/>
-    <xs:element name="TermId" type="xs:string"/>
-  </xs:schema>
-</ct:contentTypeSchema>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Owner xmlns="1e4be601-d1eb-4833-8855-b10f66ff5f6e">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId/>
-        <AccountType/>
-      </UserInfo>
-    </Owner>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e4be601-d1eb-4833-8855-b10f66ff5f6e">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{622CE4B2-692C-4431-96CF-3DD5D0902D68}"/>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7BD07885-43C3-411A-8E3F-524C132769FC}"/>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8534DFB0-209F-4F27-8B2D-2AB2E014C46E}"/>
 </file>
</xml_diff>

<commit_message>
FIX duplicate num val
</commit_message>
<xml_diff>
--- a/Comparator_Reports/Excel_Comparator/24_03_001_validation_log.xlsx
+++ b/Comparator_Reports/Excel_Comparator/24_03_001_validation_log.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="48">
   <si>
     <t>Sheet</t>
   </si>
@@ -61,13 +61,25 @@
     <t>F8</t>
   </si>
   <si>
+    <t>G8</t>
+  </si>
+  <si>
     <t>F9</t>
   </si>
   <si>
+    <t>G9</t>
+  </si>
+  <si>
     <t>F10</t>
   </si>
   <si>
+    <t>G10</t>
+  </si>
+  <si>
     <t>F11</t>
+  </si>
+  <si>
+    <t>G11</t>
   </si>
   <si>
     <t>g7</t>
@@ -503,7 +515,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -531,10 +543,10 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D2" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -545,10 +557,10 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -559,10 +571,10 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D4" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -573,10 +585,10 @@
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D5" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -587,10 +599,10 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D6" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -601,10 +613,10 @@
         <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D7" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -615,10 +627,10 @@
         <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D8" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -629,10 +641,10 @@
         <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D9" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -643,10 +655,10 @@
         <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D10" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -657,7 +669,7 @@
         <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D11" t="s">
         <v>41</v>
@@ -671,10 +683,10 @@
         <v>16</v>
       </c>
       <c r="C12" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D12" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -685,57 +697,57 @@
         <v>17</v>
       </c>
       <c r="C13" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D13" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B14" t="s">
         <v>18</v>
       </c>
       <c r="C14" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="D14" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B15" t="s">
         <v>19</v>
       </c>
       <c r="C15" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D15" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B16" t="s">
         <v>20</v>
       </c>
       <c r="C16" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="D16" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B17" t="s">
         <v>21</v>
@@ -744,7 +756,7 @@
         <v>33</v>
       </c>
       <c r="D17" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -755,10 +767,10 @@
         <v>22</v>
       </c>
       <c r="C18" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D18" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -769,10 +781,10 @@
         <v>23</v>
       </c>
       <c r="C19" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D19" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -783,10 +795,10 @@
         <v>24</v>
       </c>
       <c r="C20" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D20" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -797,10 +809,10 @@
         <v>25</v>
       </c>
       <c r="C21" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D21" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -811,10 +823,10 @@
         <v>26</v>
       </c>
       <c r="C22" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D22" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -825,13 +837,305 @@
         <v>27</v>
       </c>
       <c r="C23" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D23" t="s">
-        <v>43</v>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" t="s">
+        <v>28</v>
+      </c>
+      <c r="C24" t="s">
+        <v>35</v>
+      </c>
+      <c r="D24" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25" t="s">
+        <v>29</v>
+      </c>
+      <c r="C25" t="s">
+        <v>39</v>
+      </c>
+      <c r="D25" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26" t="s">
+        <v>35</v>
+      </c>
+      <c r="D26" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27" t="s">
+        <v>31</v>
+      </c>
+      <c r="C27" t="s">
+        <v>40</v>
+      </c>
+      <c r="D27" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004FF20ACD2ACDAF4B84EF9300C67B2159" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0c36ae600cfc71a682facb2fe9ea4a9f">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1e4be601-d1eb-4833-8855-b10f66ff5f6e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="efc49a46b45dba0aa538c93634f147fb" ns2:_="">
+    <xsd:import namespace="1e4be601-d1eb-4833-8855-b10f66ff5f6e"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns2:Owner"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="1e4be601-d1eb-4833-8855-b10f66ff5f6e" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSearchProperties" ma:index="10" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="11" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="13" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="111f8b2a-cd79-47dd-889c-3fa2f1862339" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="14" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="15" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="16" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="17" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="Owner" ma:index="18" ma:displayName="Owner" ma:format="Dropdown" ma:list="UserInfo" ma:SharePointGroup="0" ma:internalName="Owner">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Owner xmlns="1e4be601-d1eb-4833-8855-b10f66ff5f6e">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId/>
+        <AccountType/>
+      </UserInfo>
+    </Owner>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e4be601-d1eb-4833-8855-b10f66ff5f6e">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1F99717E-D820-41E5-88B6-39979FD336FB}"/>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4F9992AC-987B-4ED2-BCFA-36644DF0AC98}"/>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CCD2D186-F0A8-4280-A05B-E9367B586CF3}"/>
 </file>
</xml_diff>